<commit_message>
updating files just to have format
</commit_message>
<xml_diff>
--- a/BookingsFormat/formatToBeFollowed.xlsx
+++ b/BookingsFormat/formatToBeFollowed.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csulb-my.sharepoint.com/personal/jina_flores_csulb_edu/Documents/Documents/Data and Reports/Counseling Data/MonthlyData/WAIV/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csulb-my.sharepoint.com/personal/cdc_workability-sa1_csulb_edu/Documents/Documents/jwalitha docs/vscode program files/BookingsFormat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{855F5880-E91E-4AED-AE00-205B0E21108A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57D724CC-B0B8-4177-969F-5F16539A2311}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{855F5880-E91E-4AED-AE00-205B0E21108A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AB3F7E1-3D56-4BC2-8F7A-2598D77D31AB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-Appointments_5.1.2023_4.30.20" sheetId="1" r:id="rId1"/>
@@ -31,47 +31,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Student ID</t>
   </si>
   <si>
-    <t>Assessments</t>
-  </si>
-  <si>
     <t>10:00 AM PT</t>
   </si>
   <si>
-    <t>11:00 AM PT</t>
-  </si>
-  <si>
-    <t>Resume and Cover Letter Review</t>
-  </si>
-  <si>
-    <t>Internship/Volunteer Search</t>
-  </si>
-  <si>
     <t>Career Exploration and Planning</t>
   </si>
   <si>
-    <t>09:00 AM PT</t>
-  </si>
-  <si>
-    <t>Job Search Strategy</t>
-  </si>
-  <si>
-    <t>02:00 PM PT</t>
-  </si>
-  <si>
-    <t>12:00 PM PT</t>
-  </si>
-  <si>
-    <t>Exploring Graduate/Professional School</t>
-  </si>
-  <si>
-    <t>08:00 AM PT</t>
-  </si>
-  <si>
     <t>Counseling Type</t>
   </si>
   <si>
@@ -87,61 +57,16 @@
     <t>Counseling Time</t>
   </si>
   <si>
-    <t>Mathew Gonzales</t>
-  </si>
-  <si>
-    <t>Angi Carrillo-Humphreys</t>
-  </si>
-  <si>
-    <t>Wayne Tokunaga</t>
-  </si>
-  <si>
-    <t>In-Person</t>
-  </si>
-  <si>
     <t>Virtual</t>
   </si>
   <si>
     <t xml:space="preserve">Counselor </t>
   </si>
   <si>
-    <t>014068819</t>
-  </si>
-  <si>
-    <t>026941601</t>
-  </si>
-  <si>
-    <t>030831396</t>
-  </si>
-  <si>
-    <t>028904419</t>
-  </si>
-  <si>
-    <t>025310257</t>
-  </si>
-  <si>
-    <t>026325947</t>
-  </si>
-  <si>
-    <t>028731701</t>
-  </si>
-  <si>
-    <t>029308758</t>
-  </si>
-  <si>
-    <t>025340534</t>
-  </si>
-  <si>
-    <t>025755572</t>
-  </si>
-  <si>
-    <t>017730373</t>
-  </si>
-  <si>
-    <t>WorkAbility IV</t>
-  </si>
-  <si>
-    <t>Michelle Linton</t>
+    <t>xxxxxxxxx</t>
+  </si>
+  <si>
+    <t>CounselorName</t>
   </si>
 </sst>
 </file>
@@ -1008,7 +933,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,276 +953,86 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2">
         <v>45050</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" s="1">
         <v>60</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="2">
-        <v>45054</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1">
-        <v>30</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="D3" s="2"/>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="2">
-        <v>45054</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="1">
-        <v>30</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>20</v>
-      </c>
+      <c r="D4" s="2"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="2">
-        <v>45054</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="1">
-        <v>60</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>36</v>
-      </c>
+      <c r="D5" s="2"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="2">
-        <v>45054</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="1">
-        <v>30</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="D6" s="2"/>
+      <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="2">
-        <v>45055</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="1">
-        <v>60</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="D7" s="2"/>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="2">
-        <v>45055</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="1">
-        <v>60</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="D8" s="2"/>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="2">
-        <v>45056</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="1">
-        <v>60</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="D9" s="2"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="2">
-        <v>45056</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="1">
-        <v>60</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="D10" s="2"/>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="2">
-        <v>45057</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="1">
-        <v>60</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="D11" s="2"/>
+      <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="2">
-        <v>45057</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="1">
-        <v>30</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="D12" s="2"/>
+      <c r="G12" s="7"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G12">

</xml_diff>